<commit_message>
tugas dan prak js 8
</commit_message>
<xml_diff>
--- a/MINGGU 8/PWL_POS/public/template_barang.xlsx
+++ b/MINGGU 8/PWL_POS/public/template_barang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\s4\weblanjut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Kelas 2 Semester 2\WebLanjut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D0FFC3F-7197-40EA-9C27-0C95946DAEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA8F51D-3BB3-4F79-BE3E-C0C9EB757BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{E2BFE268-7F06-42B1-99E9-3D1AB53EDC63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E011ABB6-7838-4C25-A9AE-C084FEA0212F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>kategori_id</t>
   </si>
@@ -42,24 +42,6 @@
     <t>barang_kode</t>
   </si>
   <si>
-    <t>BK01</t>
-  </si>
-  <si>
-    <t>BK02</t>
-  </si>
-  <si>
-    <t>BK03</t>
-  </si>
-  <si>
-    <t>mmajicjer</t>
-  </si>
-  <si>
-    <t>Handphone</t>
-  </si>
-  <si>
-    <t>civic</t>
-  </si>
-  <si>
     <t>barang_nama</t>
   </si>
   <si>
@@ -67,6 +49,36 @@
   </si>
   <si>
     <t>harga_jual</t>
+  </si>
+  <si>
+    <t>BRG001</t>
+  </si>
+  <si>
+    <t>Biskuit</t>
+  </si>
+  <si>
+    <t>BRG003</t>
+  </si>
+  <si>
+    <t>Teh Botol</t>
+  </si>
+  <si>
+    <t>BRG005</t>
+  </si>
+  <si>
+    <t>Mouse Wireless</t>
+  </si>
+  <si>
+    <t>BRG007</t>
+  </si>
+  <si>
+    <t>Sapu</t>
+  </si>
+  <si>
+    <t>BRG009</t>
+  </si>
+  <si>
+    <t>Kaos Polos</t>
   </si>
 </sst>
 </file>
@@ -82,7 +94,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,8 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,92 +440,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EB10CA-F68E-4BB7-9F02-061DD76FA1D4}">
-  <dimension ref="B2:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C7E09C-F67F-4A03-912A-0D38297E12F3}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>3000</v>
+      </c>
+      <c r="E2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D3">
+        <v>2000</v>
+      </c>
+      <c r="E3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="D4">
+        <v>100000</v>
+      </c>
+      <c r="E4">
+        <v>150000</v>
+      </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="5" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>15000</v>
+      </c>
+      <c r="E5">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>500000</v>
-      </c>
-      <c r="F3">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>300000</v>
-      </c>
-      <c r="F4">
-        <v>3500000</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>5000000</v>
-      </c>
-      <c r="F5">
-        <v>75000</v>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>40000</v>
+      </c>
+      <c r="E6">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>